<commit_message>
Day 1 literature review, citation, understanding and building Graph Attention Network. Next steps identified.
</commit_message>
<xml_diff>
--- a/Literature Review.xlsx
+++ b/Literature Review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Backup_Jan30\Research\JNER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE9472E-5CF0-4D10-A93A-0AC054C4D315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593202F5-2CCE-4715-A34E-E29530A52269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
   <si>
     <r>
       <t xml:space="preserve">By downloading or using this template, you agree to comply with the </t>
@@ -400,6 +400,19 @@
   </si>
   <si>
     <t>diFuMo atlas for brain segmentation mask</t>
+  </si>
+  <si>
+    <t>{Gordić2020PyTorchGAT,
+  author = {Gordić, Aleksa},
+  title = {pytorch-GAT},
+  year = {2020},
+  publisher = {GitHub},
+  journal = {GitHub repository},
+  howpublished = {\url{https://github.com/gordicaleksa/pytorch-GAT}},
+}</t>
+  </si>
+  <si>
+    <t>GAT Implementations</t>
   </si>
 </sst>
 </file>
@@ -1462,7 +1475,7 @@
   <dimension ref="B1:L32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="70" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1702,12 +1715,16 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="2:12" ht="70" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="14"/>
+    <row r="13" spans="2:12" ht="192" x14ac:dyDescent="0.35">
+      <c r="B13" s="14" t="s">
+        <v>53</v>
+      </c>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
+      <c r="F13" s="14" t="s">
+        <v>54</v>
+      </c>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
@@ -1972,7 +1989,7 @@
     <mergeCell ref="D22:L22"/>
     <mergeCell ref="C4:H4"/>
   </mergeCells>
-  <conditionalFormatting sqref="B8:L11 B13:L21 K12:L12 B12:I12">
+  <conditionalFormatting sqref="B8:L11 B12:I12 K12:L12 B13:L21">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update 27 Feb: Literature Review update
</commit_message>
<xml_diff>
--- a/Literature Review.xlsx
+++ b/Literature Review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Backup_Jan30\Research\JNER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593202F5-2CCE-4715-A34E-E29530A52269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6A9B9F-6819-48EE-9C2F-75B62DF63630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
   <si>
     <r>
       <t xml:space="preserve">By downloading or using this template, you agree to comply with the </t>
@@ -414,12 +414,74 @@
   <si>
     <t>GAT Implementations</t>
   </si>
+  <si>
+    <t>Sui, Y., Wang, X., Wu, J., Lin, M., He, X., &amp; Chua, T.-S. (2022). Causal Attention for Interpretable and Generalizable Graph Classification. Proceedings of the 28th ACM SIGKDD Conference on Knowledge Discovery and Data Mining, 1696–1705. https://doi.org/10.1145/3534678.3539366</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Causal features and trivial features are difficult to observe from ground-truth data and therefore needed a way to identify; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Solution for identifying causal features and trivial features are learning them through manipulating attention weights of nodes and edges' features ---&gt; New Loss funciton for GAT (Lce = Lce(uniform) + Lce(supervised) + Lce(estimated causal)); </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>3.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> The estimated causal is calculated using do-calculus</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -532,6 +594,13 @@
     </font>
     <font>
       <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Century Gothic"/>
@@ -1474,14 +1543,17 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:L32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="70" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2.26953125" style="9" customWidth="1"/>
-    <col min="2" max="11" width="30.6328125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="44.6328125" style="9" customWidth="1"/>
+    <col min="3" max="5" width="30.6328125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="45.6328125" style="9" customWidth="1"/>
+    <col min="7" max="11" width="30.6328125" style="9" customWidth="1"/>
     <col min="12" max="12" width="31.1796875" style="9" customWidth="1"/>
     <col min="13" max="16384" width="8.7265625" style="9"/>
   </cols>
@@ -1732,12 +1804,16 @@
       <c r="K13" s="14"/>
       <c r="L13" s="14"/>
     </row>
-    <row r="14" spans="2:12" ht="70" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="14"/>
+    <row r="14" spans="2:12" ht="304" x14ac:dyDescent="0.35">
+      <c r="B14" s="14" t="s">
+        <v>55</v>
+      </c>
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
+      <c r="F14" s="14" t="s">
+        <v>56</v>
+      </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>

</xml_diff>